<commit_message>
Draw fittings with blocks
</commit_message>
<xml_diff>
--- a/leo_template.xlsx
+++ b/leo_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raffaello/python/planner/eurotherm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56325BA4-A000-DC41-BF62-8ABA423D34AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FE314B-5430-6C4C-B258-38ABD4B9479C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="4680" windowWidth="23460" windowHeight="8440" activeTab="2" xr2:uid="{FCD0A303-1C18-40CC-8B6D-DC148C548902}"/>
+    <workbookView xWindow="2100" yWindow="3700" windowWidth="23460" windowHeight="8440" activeTab="2" xr2:uid="{FCD0A303-1C18-40CC-8B6D-DC148C548902}"/>
   </bookViews>
   <sheets>
     <sheet name="LEONARDO 5.5" sheetId="3" r:id="rId1"/>
@@ -565,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F2F1A7B-4CB8-4234-8232-B01E47CE737E}">
   <dimension ref="A2:T5"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -674,11 +674,11 @@
       <c r="N3" s="15">
         <v>33</v>
       </c>
-      <c r="O3" s="15">
+      <c r="O3" s="16">
         <f>85*E3*D3</f>
         <v>8500</v>
       </c>
-      <c r="P3" s="15">
+      <c r="P3" s="16">
         <f>85*E3*1.1*D3</f>
         <v>9350</v>
       </c>
@@ -731,16 +731,17 @@
         <f>K4-(O4/D4/10.8)</f>
         <v>22.574074074074076</v>
       </c>
-      <c r="O4" s="15">
+      <c r="O4" s="16">
+        <f>51.8*D4*E4</f>
         <v>5180</v>
       </c>
-      <c r="P4" s="15">
-        <f>44*E4*1.1*D4</f>
-        <v>4840.0000000000009</v>
+      <c r="P4" s="16">
+        <f>51.8*E4*1.1*D4</f>
+        <v>5698</v>
       </c>
       <c r="Q4" s="16">
         <f>3.6*P4/(4.186*M4)</f>
-        <v>1664.9784997611089</v>
+        <v>1960.1337792642139</v>
       </c>
       <c r="T4" s="18"/>
     </row>
@@ -758,7 +759,7 @@
   <dimension ref="A2:T5"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -864,11 +865,11 @@
       <c r="N3" s="15">
         <v>32.9</v>
       </c>
-      <c r="O3" s="15">
+      <c r="O3" s="16">
         <f>84.2*E3*D3</f>
         <v>8420</v>
       </c>
-      <c r="P3" s="15">
+      <c r="P3" s="16">
         <f>84.2*E3*1.1*D3</f>
         <v>9262.0000000000018</v>
       </c>
@@ -921,11 +922,11 @@
         <f>K4-(O4/D4/10.8)</f>
         <v>21.714285714285715</v>
       </c>
-      <c r="O4" s="15">
+      <c r="O4" s="16">
         <f>64.8*E4*D4</f>
         <v>6480</v>
       </c>
-      <c r="P4" s="15">
+      <c r="P4" s="16">
         <f>64.8*E4*1.1*D4</f>
         <v>7128.0000000000009</v>
       </c>
@@ -947,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA07C718-141C-4F3F-A6B6-64320F3A12DA}">
   <dimension ref="A2:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -965,7 +966,7 @@
     <col min="21" max="21" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" ht="70" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="42" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1057,17 +1058,17 @@
       <c r="N3" s="15">
         <v>32.700000000000003</v>
       </c>
-      <c r="O3" s="15">
+      <c r="O3" s="16">
         <f>82.3*E3*D3</f>
         <v>8230</v>
       </c>
-      <c r="P3" s="15">
-        <f>85*E3*1.1*D3</f>
-        <v>9350</v>
+      <c r="P3" s="16">
+        <f>82.3*E3*1.1*D3</f>
+        <v>9053.0000000000018</v>
       </c>
       <c r="Q3" s="16">
         <f>3.6*P3/(4.186*M3)</f>
-        <v>2297.4540986963348</v>
+        <v>2224.4761449730399</v>
       </c>
       <c r="R3" s="17"/>
       <c r="S3" s="17"/>
@@ -1115,13 +1116,13 @@
       </c>
       <c r="N4" s="16">
         <f>K4-(O4/D4/10.8)</f>
-        <v>20.775132275132275</v>
-      </c>
-      <c r="O4" s="15">
-        <f>79*E4*D4</f>
-        <v>7900</v>
-      </c>
-      <c r="P4" s="15">
+        <v>20.649470899470899</v>
+      </c>
+      <c r="O4" s="16">
+        <f>80.9*E4*D4</f>
+        <v>8090.0000000000009</v>
+      </c>
+      <c r="P4" s="16">
         <f>80.9*E4*1.1*D4</f>
         <v>8899.0000000000018</v>
       </c>

</xml_diff>

<commit_message>
Template XLS and T/U sorted
</commit_message>
<xml_diff>
--- a/leo_template.xlsx
+++ b/leo_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raffaello/python/planner/eurotherm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B851B3C-E619-F04F-8B56-371FFA4F7C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A6B5D5-0F0D-8540-8D26-DB9D4B01D15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{FCD0A303-1C18-40CC-8B6D-DC148C548902}"/>
   </bookViews>
@@ -1205,6 +1205,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1216,21 +1231,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2023,7 +2023,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2040,10 +2040,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="82"/>
+      <c r="B1" s="87"/>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
@@ -2053,13 +2053,13 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="33"/>
       <c r="B2" s="34"/>
-      <c r="D2" s="81" t="s">
+      <c r="D2" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
       <c r="J2" s="58"/>
       <c r="K2" s="59"/>
       <c r="L2" s="59"/>
@@ -2070,12 +2070,12 @@
       <c r="A3" s="35"/>
       <c r="B3" s="36"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="81" t="s">
+      <c r="E3" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
       <c r="J3" s="61"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -2087,12 +2087,12 @@
       <c r="A4" s="35"/>
       <c r="B4" s="36"/>
       <c r="D4" s="39"/>
-      <c r="E4" s="83" t="s">
+      <c r="E4" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
       <c r="J4" s="61"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -2103,12 +2103,12 @@
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="35"/>
       <c r="B5" s="36"/>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
       <c r="H5" s="40"/>
       <c r="J5" s="63"/>
       <c r="K5" s="4"/>
@@ -2120,12 +2120,12 @@
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="35"/>
       <c r="B6" s="36"/>
-      <c r="D6" s="81" t="s">
+      <c r="D6" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="81"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
       <c r="H6" s="4"/>
       <c r="J6" s="61"/>
       <c r="K6" s="4"/>
@@ -2136,12 +2136,12 @@
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="35"/>
       <c r="B7" s="36"/>
-      <c r="D7" s="80" t="s">
+      <c r="D7" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
       <c r="H7" s="41"/>
       <c r="J7" s="61"/>
       <c r="K7" s="4"/>
@@ -2153,12 +2153,12 @@
       <c r="A8" s="37"/>
       <c r="B8" s="38"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="81" t="s">
+      <c r="D8" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
       <c r="H8" s="40"/>
       <c r="J8" s="64"/>
       <c r="K8" s="65"/>
@@ -2233,17 +2233,17 @@
       <c r="P13" s="67"/>
     </row>
     <row r="14" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="86">
+      <c r="A14" s="82">
         <v>100</v>
       </c>
-      <c r="B14" s="86">
+      <c r="B14" s="82">
         <v>140</v>
       </c>
-      <c r="C14" s="84">
+      <c r="C14" s="80">
         <f>A14/B14</f>
         <v>0.7142857142857143</v>
       </c>
-      <c r="D14" s="48"/>
+      <c r="D14" s="49"/>
       <c r="E14" s="47"/>
       <c r="F14" s="49">
         <f>_xlfn.CEILING.MATH(B14/10,1)</f>
@@ -2334,13 +2334,13 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="88">
+      <c r="A18" s="84">
         <v>100</v>
       </c>
-      <c r="B18" s="87">
+      <c r="B18" s="83">
         <v>140</v>
       </c>
-      <c r="C18" s="85">
+      <c r="C18" s="81">
         <f>A18/B18</f>
         <v>0.7142857142857143</v>
       </c>
@@ -2421,10 +2421,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="82"/>
+      <c r="B1" s="87"/>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
@@ -2435,13 +2435,13 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="33"/>
       <c r="B2" s="34"/>
-      <c r="D2" s="81" t="s">
+      <c r="D2" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
       <c r="J2" s="73"/>
       <c r="K2" s="74"/>
       <c r="L2" s="74"/>
@@ -2452,12 +2452,12 @@
       <c r="A3" s="35"/>
       <c r="B3" s="36"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="81" t="s">
+      <c r="E3" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
       <c r="I3" s="4"/>
       <c r="J3" s="76"/>
       <c r="K3" s="4"/>
@@ -2470,12 +2470,12 @@
       <c r="A4" s="35"/>
       <c r="B4" s="36"/>
       <c r="D4" s="39"/>
-      <c r="E4" s="83" t="s">
+      <c r="E4" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
       <c r="I4" s="4"/>
       <c r="J4" s="76"/>
       <c r="K4" s="4"/>
@@ -2487,12 +2487,12 @@
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="35"/>
       <c r="B5" s="36"/>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
       <c r="H5" s="40"/>
       <c r="I5" s="4"/>
       <c r="J5" s="76"/>
@@ -2505,12 +2505,12 @@
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="35"/>
       <c r="B6" s="36"/>
-      <c r="D6" s="81" t="s">
+      <c r="D6" s="86" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="81"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="76"/>
@@ -2522,12 +2522,12 @@
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="35"/>
       <c r="B7" s="36"/>
-      <c r="D7" s="80" t="s">
+      <c r="D7" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
       <c r="H7" s="41"/>
       <c r="I7" s="4"/>
       <c r="J7" s="76"/>
@@ -2540,12 +2540,12 @@
       <c r="A8" s="37"/>
       <c r="B8" s="38"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="81" t="s">
+      <c r="D8" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
       <c r="H8" s="40"/>
       <c r="J8" s="77"/>
       <c r="K8" s="78"/>
@@ -2811,10 +2811,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="82"/>
+      <c r="B1" s="87"/>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
@@ -2824,13 +2824,13 @@
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="33"/>
       <c r="B2" s="34"/>
-      <c r="D2" s="81" t="s">
+      <c r="D2" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
       <c r="J2" s="73"/>
       <c r="K2" s="74"/>
       <c r="L2" s="74"/>
@@ -2841,12 +2841,12 @@
       <c r="A3" s="35"/>
       <c r="B3" s="36"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="81" t="s">
+      <c r="E3" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
       <c r="J3" s="76"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -2861,12 +2861,12 @@
       <c r="A4" s="35"/>
       <c r="B4" s="36"/>
       <c r="D4" s="39"/>
-      <c r="E4" s="83" t="s">
+      <c r="E4" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
       <c r="J4" s="76"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -2880,12 +2880,12 @@
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="35"/>
       <c r="B5" s="36"/>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
       <c r="H5" s="40"/>
       <c r="J5" s="76"/>
       <c r="K5" s="4"/>
@@ -2903,12 +2903,12 @@
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="35"/>
       <c r="B6" s="36"/>
-      <c r="D6" s="81" t="s">
+      <c r="D6" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="81"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
       <c r="H6" s="4"/>
       <c r="J6" s="76"/>
       <c r="K6" s="4"/>
@@ -2921,12 +2921,12 @@
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="35"/>
       <c r="B7" s="36"/>
-      <c r="D7" s="80" t="s">
+      <c r="D7" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
       <c r="H7" s="41"/>
       <c r="J7" s="76"/>
       <c r="K7" s="4"/>
@@ -2938,12 +2938,12 @@
       <c r="A8" s="37"/>
       <c r="B8" s="38"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="81" t="s">
+      <c r="D8" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
       <c r="H8" s="40"/>
       <c r="J8" s="77"/>
       <c r="K8" s="78"/>

</xml_diff>

<commit_message>
Template fix with images (using pillow)
</commit_message>
<xml_diff>
--- a/leo_template.xlsx
+++ b/leo_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raffaello/python/planner/eurotherm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raffaello/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A6B5D5-0F0D-8540-8D26-DB9D4B01D15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2A7BBF-B8E2-B94C-85CC-06E4710188C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{FCD0A303-1C18-40CC-8B6D-DC148C548902}"/>
   </bookViews>
@@ -1056,15 +1056,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1101,9 +1098,8 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1126,12 +1122,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
@@ -1171,10 +1167,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
@@ -1193,7 +1189,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1205,12 +1201,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1223,10 +1213,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1721,7 +1711,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2009,7 +1999,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2023,7 +2013,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2040,345 +2030,323 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="B1" s="81"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="33"/>
-      <c r="B2" s="34"/>
-      <c r="D2" s="86" t="s">
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="D2" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="60"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="56"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="86" t="s">
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="E3" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="62"/>
-      <c r="T3" s="2"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="J3" s="57"/>
+      <c r="N3" s="58"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="88" t="s">
+      <c r="A4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="62"/>
-      <c r="T4" s="2"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="J4" s="57"/>
+      <c r="N4" s="58"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="35"/>
-      <c r="B5" s="36"/>
-      <c r="D5" s="85" t="s">
+      <c r="A5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="D5" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="40"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="62"/>
-      <c r="T5" s="3"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="36"/>
+      <c r="J5" s="59"/>
+      <c r="N5" s="58"/>
+      <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
-      <c r="B6" s="36"/>
-      <c r="D6" s="86" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="32"/>
+      <c r="D6" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="4"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="62"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="J6" s="57"/>
+      <c r="N6" s="58"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="35"/>
-      <c r="B7" s="36"/>
-      <c r="D7" s="85" t="s">
+      <c r="A7" s="31"/>
+      <c r="B7" s="32"/>
+      <c r="D7" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="41"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="62"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="37"/>
+      <c r="J7" s="57"/>
+      <c r="N7" s="58"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="86" t="s">
+      <c r="A8" s="33"/>
+      <c r="B8" s="34"/>
+      <c r="D8" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="40"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
-      <c r="N8" s="66"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="36"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="62"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="J13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="M13" s="7" t="s">
+      <c r="M13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="10" t="s">
+      <c r="N13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O13" s="68" t="s">
+      <c r="O13" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="P13" s="67"/>
+      <c r="P13" s="63"/>
     </row>
     <row r="14" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="82">
+      <c r="A14" s="76">
         <v>100</v>
       </c>
-      <c r="B14" s="82">
+      <c r="B14" s="76">
         <v>140</v>
       </c>
-      <c r="C14" s="80">
+      <c r="C14" s="44">
         <f>A14/B14</f>
         <v>0.7142857142857143</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="49">
+      <c r="D14" s="45"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="45">
         <f>_xlfn.CEILING.MATH(B14/10,1)</f>
         <v>14</v>
       </c>
-      <c r="G14" s="48">
+      <c r="G14" s="44">
         <f>IF(F14&gt;8,_xlfn.CEILING.MATH(F14/8),"1")</f>
         <v>2</v>
       </c>
-      <c r="H14" s="47">
+      <c r="H14" s="43">
         <v>300</v>
       </c>
-      <c r="I14" s="49">
+      <c r="I14" s="45">
         <v>20</v>
       </c>
-      <c r="J14" s="48">
+      <c r="J14" s="45">
         <v>43</v>
       </c>
-      <c r="K14" s="47">
+      <c r="K14" s="43">
         <v>3.5</v>
       </c>
-      <c r="L14" s="49">
+      <c r="L14" s="45">
         <v>33</v>
       </c>
-      <c r="M14" s="48">
+      <c r="M14" s="45">
         <f>85*C14*B14</f>
         <v>8500</v>
       </c>
-      <c r="N14" s="47">
+      <c r="N14" s="43">
         <f>85*C14*1.1*B14</f>
         <v>9350</v>
       </c>
-      <c r="O14" s="49">
+      <c r="O14" s="45">
         <f>3.6*N14/(4.186*K14)</f>
         <v>2297.4540986963348</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="70" t="s">
+      <c r="A16" s="66" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="43.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="71" t="s">
+      <c r="A17" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="J17" s="11" t="s">
+      <c r="J17" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="K17" s="11" t="s">
+      <c r="K17" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="L17" s="11" t="s">
+      <c r="L17" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="M17" s="11" t="s">
+      <c r="M17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N17" s="11" t="s">
+      <c r="N17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O17" s="11" t="s">
+      <c r="O17" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="84">
+      <c r="A18" s="78">
         <v>100</v>
       </c>
-      <c r="B18" s="83">
+      <c r="B18" s="77">
         <v>140</v>
       </c>
-      <c r="C18" s="81">
+      <c r="C18" s="13">
         <f>A18/B18</f>
         <v>0.7142857142857143</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18">
+      <c r="D18" s="15"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15">
         <f>_xlfn.CEILING.MATH(B18/10,1)</f>
         <v>14</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="14">
         <f>IF(F18&gt;8,_xlfn.CEILING.MATH(F18/8),"1")</f>
         <v>2</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="15">
         <v>300</v>
       </c>
-      <c r="I18" s="17">
+      <c r="I18" s="14">
         <v>26</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="15">
         <v>14</v>
       </c>
-      <c r="K18" s="17">
+      <c r="K18" s="14">
         <v>2.5</v>
       </c>
-      <c r="L18" s="18">
+      <c r="L18" s="15">
         <f>I18-(M18/B18/10.8)</f>
         <v>22.574074074074076</v>
       </c>
-      <c r="M18" s="17">
+      <c r="M18" s="14">
         <f>51.8*B18*C18</f>
         <v>5180</v>
       </c>
-      <c r="N18" s="18">
+      <c r="N18" s="15">
         <f>51.8*C18*1.1*B18</f>
         <v>5698</v>
       </c>
-      <c r="O18" s="17">
+      <c r="O18" s="14">
         <f>3.6*N18/(4.186*K18)</f>
         <v>1960.1337792642139</v>
       </c>
@@ -2421,350 +2389,322 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="J1" s="4"/>
+      <c r="B1" s="81"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="33"/>
-      <c r="B2" s="34"/>
-      <c r="D2" s="86" t="s">
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="D2" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="75"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="71"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="86" t="s">
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="E3" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="72"/>
-      <c r="T3" s="2"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="J3" s="72"/>
+      <c r="N3" s="68"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="88" t="s">
+      <c r="A4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="72"/>
-      <c r="T4" s="2"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="J4" s="72"/>
+      <c r="N4" s="68"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="35"/>
-      <c r="B5" s="36"/>
-      <c r="D5" s="85" t="s">
+      <c r="A5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="D5" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="72"/>
-      <c r="T5" s="3"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="36"/>
+      <c r="J5" s="72"/>
+      <c r="N5" s="68"/>
+      <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
-      <c r="B6" s="36"/>
-      <c r="D6" s="86" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="32"/>
+      <c r="D6" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="72"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="J6" s="72"/>
+      <c r="N6" s="68"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="35"/>
-      <c r="B7" s="36"/>
-      <c r="D7" s="85" t="s">
+      <c r="A7" s="31"/>
+      <c r="B7" s="32"/>
+      <c r="D7" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="72"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="37"/>
+      <c r="J7" s="72"/>
+      <c r="N7" s="68"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="86" t="s">
+      <c r="A8" s="33"/>
+      <c r="B8" s="34"/>
+      <c r="D8" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="40"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="79"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="36"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="75"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="52" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="43.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="42" t="s">
+      <c r="H13" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="43" t="s">
+      <c r="K13" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="L13" s="44" t="s">
+      <c r="L13" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="M13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="43" t="s">
+      <c r="N13" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="O13" s="9" t="s">
+      <c r="O13" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45">
+      <c r="A14" s="41">
         <v>100</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B14" s="42">
         <v>140</v>
       </c>
-      <c r="C14" s="48">
+      <c r="C14" s="44">
         <f>A14/B14</f>
         <v>0.7142857142857143</v>
       </c>
-      <c r="D14" s="47"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="50">
+      <c r="D14" s="43"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="46">
         <f>_xlfn.CEILING.MATH(B14/10,1)</f>
         <v>14</v>
       </c>
-      <c r="G14" s="51">
+      <c r="G14" s="47">
         <f>IF(F14&gt;8,_xlfn.CEILING.MATH(F14/8),"1")</f>
         <v>2</v>
       </c>
-      <c r="H14" s="52">
+      <c r="H14" s="48">
         <v>300</v>
       </c>
-      <c r="I14" s="53">
+      <c r="I14" s="49">
         <v>20</v>
       </c>
-      <c r="J14" s="53">
+      <c r="J14" s="49">
         <v>39.5</v>
       </c>
-      <c r="K14" s="53">
+      <c r="K14" s="49">
         <v>3.5</v>
       </c>
-      <c r="L14" s="53">
+      <c r="L14" s="49">
         <v>32.9</v>
       </c>
-      <c r="M14" s="54">
+      <c r="M14" s="50">
         <f>84.2*C14*B14</f>
         <v>8420</v>
       </c>
-      <c r="N14" s="54">
+      <c r="N14" s="50">
         <f>84.2*C14*1.1*B14</f>
         <v>9262.0000000000018</v>
       </c>
-      <c r="O14" s="55">
+      <c r="O14" s="51">
         <f>3.6*N14/(4.186*K14)</f>
         <v>2275.83100129684</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="53" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="43.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="I17" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="L17" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="M17" s="25" t="s">
+      <c r="M17" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="N17" s="28" t="s">
+      <c r="N17" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="O17" s="26" t="s">
+      <c r="O17" s="22" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30">
+      <c r="A18" s="26">
         <v>100</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="25">
         <v>140</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="13">
         <f>A18/B18</f>
         <v>0.7142857142857143</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18">
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15">
         <f>_xlfn.CEILING.MATH(B18/10,1)</f>
         <v>14</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="15">
         <f>IF(F18&gt;8,_xlfn.CEILING.MATH(F18/8),"1")</f>
         <v>2</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="15">
         <v>300</v>
       </c>
-      <c r="I18" s="15">
+      <c r="I18" s="12">
         <v>26</v>
       </c>
-      <c r="J18" s="15">
+      <c r="J18" s="12">
         <v>14</v>
       </c>
-      <c r="K18" s="15">
+      <c r="K18" s="12">
         <v>3</v>
       </c>
-      <c r="L18" s="19">
+      <c r="L18" s="16">
         <f>I18-(M18/B18/10.8)</f>
         <v>21.714285714285715</v>
       </c>
-      <c r="M18" s="20">
+      <c r="M18" s="17">
         <f>64.8*C18*B18</f>
         <v>6480</v>
       </c>
-      <c r="N18" s="27">
+      <c r="N18" s="23">
         <f>64.8*C18*1.1*B18</f>
         <v>7128.0000000000009</v>
       </c>
-      <c r="O18" s="21">
+      <c r="O18" s="18">
         <f>3.6*N18/(4.186*K18)</f>
         <v>2043.3827042522698</v>
       </c>
@@ -2790,7 +2730,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O8" sqref="O8"/>
@@ -2810,376 +2750,338 @@
     <col min="21" max="21" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+    <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="33"/>
-      <c r="B2" s="34"/>
-      <c r="D2" s="86" t="s">
+      <c r="B1" s="81"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="D2" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="75"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="86" t="s">
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="71"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="E3" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="72"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="4"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="88" t="s">
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="J3" s="72"/>
+      <c r="N3" s="68"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="72"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="4"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="35"/>
-      <c r="B5" s="36"/>
-      <c r="D5" s="85" t="s">
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="J4" s="72"/>
+      <c r="N4" s="68"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="D5" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="40"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="4"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
-      <c r="B6" s="36"/>
-      <c r="D6" s="86" t="s">
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="36"/>
+      <c r="J5" s="72"/>
+      <c r="N5" s="68"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="31"/>
+      <c r="B6" s="32"/>
+      <c r="D6" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="4"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="72"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" s="35"/>
-      <c r="B7" s="36"/>
-      <c r="D7" s="85" t="s">
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="J6" s="72"/>
+      <c r="N6" s="68"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="31"/>
+      <c r="B7" s="32"/>
+      <c r="D7" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="41"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="72"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="86" t="s">
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="37"/>
+      <c r="J7" s="72"/>
+      <c r="N7" s="68"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="33"/>
+      <c r="B8" s="34"/>
+      <c r="D8" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="40"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="79"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-    </row>
-    <row r="10" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="36"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="75"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+    </row>
+    <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="4"/>
-    </row>
-    <row r="13" spans="1:21" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:20" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="42" t="s">
+      <c r="H13" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="43" t="s">
+      <c r="K13" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="L13" s="44" t="s">
+      <c r="L13" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="M13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="43" t="s">
+      <c r="N13" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="O13" s="9" t="s">
+      <c r="O13" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45">
+    <row r="14" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="41">
         <v>100</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B14" s="42">
         <v>140</v>
       </c>
-      <c r="C14" s="48">
+      <c r="C14" s="44">
         <f>A14/B14</f>
         <v>0.7142857142857143</v>
       </c>
-      <c r="D14" s="47"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="50">
+      <c r="D14" s="43"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="46">
         <f>_xlfn.CEILING.MATH(B14/10,1)</f>
         <v>14</v>
       </c>
-      <c r="G14" s="51">
+      <c r="G14" s="47">
         <f>IF(F14&gt;8,_xlfn.CEILING.MATH(F14/8),"1")</f>
         <v>2</v>
       </c>
-      <c r="H14" s="52">
+      <c r="H14" s="48">
         <v>300</v>
       </c>
-      <c r="I14" s="53">
+      <c r="I14" s="49">
         <v>20</v>
       </c>
-      <c r="J14" s="53">
+      <c r="J14" s="49">
         <v>37.5</v>
       </c>
-      <c r="K14" s="53">
+      <c r="K14" s="49">
         <v>3.5</v>
       </c>
-      <c r="L14" s="53">
+      <c r="L14" s="49">
         <v>32.700000000000003</v>
       </c>
-      <c r="M14" s="54">
+      <c r="M14" s="50">
         <f>82.3*C14*B14</f>
         <v>8230</v>
       </c>
-      <c r="N14" s="54">
+      <c r="N14" s="50">
         <f>82.3*C14*1.1*B14</f>
         <v>9053.0000000000018</v>
       </c>
-      <c r="O14" s="55">
+      <c r="O14" s="51">
         <f>3.6*N14/(4.186*K14)</f>
         <v>2224.4761449730399</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+    <row r="16" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="O16" s="14"/>
-      <c r="P16" s="4"/>
+      <c r="O16" s="11"/>
     </row>
     <row r="17" spans="1:15" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="I17" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="L17" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="M17" s="25" t="s">
+      <c r="M17" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="N17" s="28" t="s">
+      <c r="N17" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="O17" s="26" t="s">
+      <c r="O17" s="22" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30">
+      <c r="A18" s="26">
         <v>100</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="25">
         <v>140</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="13">
         <f>A18/B18</f>
         <v>0.7142857142857143</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18">
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15">
         <f>_xlfn.CEILING.MATH(B18/10,1)</f>
         <v>14</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="15">
         <f>IF(F18&gt;8,_xlfn.CEILING.MATH(F18/8),"1")</f>
         <v>2</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="15">
         <v>300</v>
       </c>
-      <c r="I18" s="15">
+      <c r="I18" s="12">
         <v>26</v>
       </c>
-      <c r="J18" s="15">
+      <c r="J18" s="12">
         <v>14</v>
       </c>
-      <c r="K18" s="15">
+      <c r="K18" s="12">
         <v>3.5</v>
       </c>
-      <c r="L18" s="19">
+      <c r="L18" s="16">
         <f>I18-(M18/B18/10.8)</f>
         <v>20.649470899470899</v>
       </c>
-      <c r="M18" s="20">
+      <c r="M18" s="17">
         <f>80.9*C18*B18</f>
         <v>8090.0000000000009</v>
       </c>
-      <c r="N18" s="27">
+      <c r="N18" s="23">
         <f>80.9*C18*1.1*B18</f>
         <v>8899.0000000000018</v>
       </c>
-      <c r="O18" s="21">
+      <c r="O18" s="18">
         <f>3.6*N18/(4.186*K18)</f>
         <v>2186.6357245239237</v>
       </c>

</xml_diff>

<commit_message>
Adding formulas to XLS
</commit_message>
<xml_diff>
--- a/leo_template.xlsx
+++ b/leo_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raffaello/python/planner/eurotherm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1C46F6-EF23-4147-B7D0-B6FD210E5EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA61604E-5D6D-5045-82E7-CA0CF39C64A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24900" windowHeight="12580" activeTab="2" xr2:uid="{FCD0A303-1C18-40CC-8B6D-DC148C548902}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24780" windowHeight="12580" activeTab="2" xr2:uid="{FCD0A303-1C18-40CC-8B6D-DC148C548902}"/>
   </bookViews>
   <sheets>
     <sheet name="LEONARDO 5.5" sheetId="3" r:id="rId1"/>
@@ -1218,6 +1218,9 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1229,9 +1232,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2023,8 +2023,8 @@
   </sheetPr>
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P10" sqref="P1:P1048576"/>
+    <sheetView topLeftCell="A5" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2042,10 +2042,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="80"/>
+      <c r="B1" s="81"/>
       <c r="D1" s="35"/>
       <c r="E1" s="35"/>
       <c r="F1" s="35"/>
@@ -2055,13 +2055,13 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="29"/>
       <c r="B2" s="30"/>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
       <c r="J2" s="54"/>
       <c r="K2" s="55"/>
       <c r="L2" s="55"/>
@@ -2071,12 +2071,12 @@
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="31"/>
       <c r="B3" s="32"/>
-      <c r="E3" s="79" t="s">
+      <c r="E3" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
       <c r="J3" s="57"/>
       <c r="N3" s="58"/>
     </row>
@@ -2084,24 +2084,24 @@
       <c r="A4" s="31"/>
       <c r="B4" s="32"/>
       <c r="D4" s="35"/>
-      <c r="E4" s="81" t="s">
+      <c r="E4" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
       <c r="J4" s="57"/>
       <c r="N4" s="58"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="31"/>
       <c r="B5" s="32"/>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
       <c r="H5" s="36"/>
       <c r="J5" s="59"/>
       <c r="N5" s="58"/>
@@ -2110,24 +2110,24 @@
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="31"/>
       <c r="B6" s="32"/>
-      <c r="D6" s="79" t="s">
+      <c r="D6" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
       <c r="J6" s="57"/>
       <c r="N6" s="58"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="31"/>
       <c r="B7" s="32"/>
-      <c r="D7" s="78" t="s">
+      <c r="D7" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
       <c r="H7" s="37"/>
       <c r="J7" s="57"/>
       <c r="N7" s="58"/>
@@ -2135,12 +2135,12 @@
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="33"/>
       <c r="B8" s="34"/>
-      <c r="D8" s="79" t="s">
+      <c r="D8" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
       <c r="H8" s="36"/>
       <c r="J8" s="60"/>
       <c r="K8" s="61"/>
@@ -2210,7 +2210,7 @@
       <c r="O13" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="P13" s="82" t="s">
+      <c r="P13" s="78" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2262,7 +2262,10 @@
         <f>3.6*N14/(4.186*K14)</f>
         <v>2297.4540986963348</v>
       </c>
-      <c r="P14" s="45"/>
+      <c r="P14" s="45">
+        <f>0.043*A14*16.67+0.41*B14</f>
+        <v>129.08099999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="65" t="s">
@@ -2368,7 +2371,10 @@
         <f>3.6*N18/(4.186*K18)</f>
         <v>1960.1337792642139</v>
       </c>
-      <c r="P18" s="14"/>
+      <c r="P18" s="14">
+        <f>0.043*A14*16.67+0.41*B14</f>
+        <v>129.08099999999999</v>
+      </c>
     </row>
     <row r="21" spans="1:16" ht="43.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -2393,7 +2399,7 @@
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2409,10 +2415,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="80"/>
+      <c r="B1" s="81"/>
       <c r="D1" s="35"/>
       <c r="E1" s="35"/>
       <c r="F1" s="35"/>
@@ -2422,13 +2428,13 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="29"/>
       <c r="B2" s="30"/>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
       <c r="J2" s="68"/>
       <c r="K2" s="69"/>
       <c r="L2" s="69"/>
@@ -2438,12 +2444,12 @@
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="31"/>
       <c r="B3" s="32"/>
-      <c r="E3" s="79" t="s">
+      <c r="E3" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
       <c r="J3" s="71"/>
       <c r="N3" s="67"/>
     </row>
@@ -2451,24 +2457,24 @@
       <c r="A4" s="31"/>
       <c r="B4" s="32"/>
       <c r="D4" s="35"/>
-      <c r="E4" s="81" t="s">
+      <c r="E4" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
       <c r="J4" s="71"/>
       <c r="N4" s="67"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="31"/>
       <c r="B5" s="32"/>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
       <c r="H5" s="36"/>
       <c r="J5" s="71"/>
       <c r="N5" s="67"/>
@@ -2477,24 +2483,24 @@
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="31"/>
       <c r="B6" s="32"/>
-      <c r="D6" s="79" t="s">
+      <c r="D6" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
       <c r="J6" s="71"/>
       <c r="N6" s="67"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="31"/>
       <c r="B7" s="32"/>
-      <c r="D7" s="78" t="s">
+      <c r="D7" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
       <c r="H7" s="37"/>
       <c r="J7" s="71"/>
       <c r="N7" s="67"/>
@@ -2502,12 +2508,12 @@
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="33"/>
       <c r="B8" s="34"/>
-      <c r="D8" s="79" t="s">
+      <c r="D8" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
       <c r="H8" s="36"/>
       <c r="J8" s="72"/>
       <c r="K8" s="73"/>
@@ -2577,7 +2583,7 @@
       <c r="O13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P13" s="82" t="s">
+      <c r="P13" s="78" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2629,7 +2635,10 @@
         <f>3.6*N14/(4.186*K14)</f>
         <v>2275.83100129684</v>
       </c>
-      <c r="P14" s="45"/>
+      <c r="P14" s="45">
+        <f>0.043*A14*23.34+0.41*B14</f>
+        <v>157.762</v>
+      </c>
     </row>
     <row r="16" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="53" t="s">
@@ -2735,7 +2744,10 @@
         <f>3.6*N18/(4.186*K18)</f>
         <v>2043.3827042522698</v>
       </c>
-      <c r="P18" s="14"/>
+      <c r="P18" s="14">
+        <f>0.043*A14*23.34+0.41*B14</f>
+        <v>157.762</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2760,8 +2772,8 @@
   </sheetPr>
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2779,10 +2791,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="80"/>
+      <c r="B1" s="81"/>
       <c r="D1" s="35"/>
       <c r="E1" s="35"/>
       <c r="F1" s="35"/>
@@ -2792,13 +2804,13 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="29"/>
       <c r="B2" s="30"/>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
       <c r="J2" s="68"/>
       <c r="K2" s="69"/>
       <c r="L2" s="69"/>
@@ -2808,12 +2820,12 @@
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="31"/>
       <c r="B3" s="32"/>
-      <c r="E3" s="79" t="s">
+      <c r="E3" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
       <c r="J3" s="71"/>
       <c r="N3" s="67"/>
     </row>
@@ -2821,24 +2833,24 @@
       <c r="A4" s="31"/>
       <c r="B4" s="32"/>
       <c r="D4" s="35"/>
-      <c r="E4" s="81" t="s">
+      <c r="E4" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
       <c r="J4" s="71"/>
       <c r="N4" s="67"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="31"/>
       <c r="B5" s="32"/>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
       <c r="H5" s="36"/>
       <c r="J5" s="71"/>
       <c r="N5" s="67"/>
@@ -2847,24 +2859,24 @@
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="31"/>
       <c r="B6" s="32"/>
-      <c r="D6" s="79" t="s">
+      <c r="D6" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
       <c r="J6" s="71"/>
       <c r="N6" s="67"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="31"/>
       <c r="B7" s="32"/>
-      <c r="D7" s="78" t="s">
+      <c r="D7" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
       <c r="H7" s="37"/>
       <c r="J7" s="71"/>
       <c r="N7" s="67"/>
@@ -2872,12 +2884,12 @@
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="33"/>
       <c r="B8" s="34"/>
-      <c r="D8" s="79" t="s">
+      <c r="D8" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
       <c r="H8" s="36"/>
       <c r="J8" s="72"/>
       <c r="K8" s="73"/>
@@ -2961,7 +2973,7 @@
       <c r="O13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="P13" s="82" t="s">
+      <c r="P13" s="78" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3013,7 +3025,10 @@
         <f>3.6*N14/(4.186*K14)</f>
         <v>2224.4761449730399</v>
       </c>
-      <c r="P14" s="45"/>
+      <c r="P14" s="45">
+        <f>0.043*A14*27.5+0.41*B14</f>
+        <v>175.65</v>
+      </c>
     </row>
     <row r="16" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
@@ -3120,7 +3135,10 @@
         <f>3.6*N18/(4.186*K18)</f>
         <v>2186.6357245239237</v>
       </c>
-      <c r="P18" s="14"/>
+      <c r="P18" s="14">
+        <f>0.043*A14*27.5+0.41*B14</f>
+        <v>175.65</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
XLS looks better now
</commit_message>
<xml_diff>
--- a/leo_template.xlsx
+++ b/leo_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raffaello/python/planner/eurotherm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eng863\Desktop\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E527B631-D441-6648-8F24-A40EC02E02DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D243464E-65C0-405A-829A-41AA8E953E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24780" windowHeight="12580" xr2:uid="{FCD0A303-1C18-40CC-8B6D-DC148C548902}"/>
+    <workbookView xWindow="2700" yWindow="810" windowWidth="25035" windowHeight="13635" xr2:uid="{FCD0A303-1C18-40CC-8B6D-DC148C548902}"/>
   </bookViews>
   <sheets>
     <sheet name="LEONARDO 5.5" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="38">
   <si>
     <t>Tamb
 °C</t>
@@ -368,9 +368,6 @@
     </r>
   </si>
   <si>
-    <t>Portata totale inriscaldamento kg/h</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -450,6 +447,13 @@
   </si>
   <si>
     <t>Contenuto d'acqua l</t>
+  </si>
+  <si>
+    <t>Portata totale in raffrescamento
+kg/h</t>
+  </si>
+  <si>
+    <t>Portata totale in raffrescamento kg/h</t>
   </si>
 </sst>
 </file>
@@ -1236,7 +1240,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1268,8 +1272,8 @@
       <xdr:rowOff>170180</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1051560</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>10160</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>12699</xdr:rowOff>
     </xdr:to>
@@ -1318,7 +1322,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>518161</xdr:colOff>
+      <xdr:colOff>594361</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
@@ -1422,8 +1426,8 @@
       <xdr:rowOff>170180</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1051560</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>13335</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>12699</xdr:rowOff>
     </xdr:to>
@@ -1472,7 +1476,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>518161</xdr:colOff>
+      <xdr:colOff>594361</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
@@ -1576,8 +1580,8 @@
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1051560</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>13335</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
@@ -1627,7 +1631,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>518161</xdr:colOff>
+      <xdr:colOff>594361</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
@@ -1722,9 +1726,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1762,7 +1766,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1868,7 +1872,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2010,7 +2014,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2023,27 +2027,27 @@
   </sheetPr>
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="7" width="9.83203125" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" customWidth="1"/>
-    <col min="9" max="14" width="9.83203125" customWidth="1"/>
-    <col min="15" max="15" width="17.83203125" customWidth="1"/>
-    <col min="16" max="16" width="14.83203125" customWidth="1"/>
-    <col min="17" max="17" width="12.5" customWidth="1"/>
-    <col min="18" max="18" width="2.33203125" customWidth="1"/>
-    <col min="19" max="19" width="2.5" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" customWidth="1"/>
+    <col min="1" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="14" width="9.85546875" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" customWidth="1"/>
+    <col min="18" max="18" width="2.28515625" customWidth="1"/>
+    <col min="19" max="19" width="2.42578125" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="81" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="81"/>
       <c r="D1" s="35"/>
@@ -2052,7 +2056,7 @@
       <c r="G1" s="35"/>
       <c r="H1" s="35"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
       <c r="B2" s="30"/>
       <c r="D2" s="80" t="s">
@@ -2068,7 +2072,7 @@
       <c r="M2" s="55"/>
       <c r="N2" s="56"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
       <c r="B3" s="32"/>
       <c r="E3" s="80" t="s">
@@ -2080,7 +2084,7 @@
       <c r="J3" s="57"/>
       <c r="N3" s="58"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" s="32"/>
       <c r="D4" s="35"/>
@@ -2093,7 +2097,7 @@
       <c r="J4" s="57"/>
       <c r="N4" s="58"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="32"/>
       <c r="D5" s="79" t="s">
@@ -2107,11 +2111,11 @@
       <c r="N5" s="58"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="32"/>
       <c r="D6" s="80" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="80"/>
       <c r="F6" s="80"/>
@@ -2119,11 +2123,11 @@
       <c r="J6" s="57"/>
       <c r="N6" s="58"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="32"/>
       <c r="D7" s="79" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="79"/>
       <c r="F7" s="79"/>
@@ -2132,7 +2136,7 @@
       <c r="J7" s="57"/>
       <c r="N7" s="58"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="33"/>
       <c r="B8" s="34"/>
       <c r="D8" s="80" t="s">
@@ -2148,23 +2152,23 @@
       <c r="M8" s="61"/>
       <c r="N8" s="62"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="45.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="64" t="s">
         <v>9</v>
       </c>
@@ -2211,10 +2215,10 @@
         <v>4</v>
       </c>
       <c r="P13" s="78" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="75">
         <v>100</v>
       </c>
@@ -2267,12 +2271,12 @@
         <v>129.08099999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="65" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="43.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="45.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="66" t="s">
         <v>9</v>
       </c>
@@ -2316,13 +2320,13 @@
         <v>13</v>
       </c>
       <c r="O17" s="8" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="77">
         <v>100</v>
       </c>
@@ -2376,7 +2380,7 @@
         <v>129.08099999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="43.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:16" ht="43.7" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="D7:G7"/>
@@ -2399,24 +2403,24 @@
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="7" width="9.83203125" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" customWidth="1"/>
-    <col min="9" max="14" width="9.83203125" customWidth="1"/>
-    <col min="15" max="15" width="17.83203125" customWidth="1"/>
-    <col min="16" max="16" width="14.83203125" customWidth="1"/>
-    <col min="18" max="19" width="2.33203125" customWidth="1"/>
-    <col min="21" max="21" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="14" width="9.85546875" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" customWidth="1"/>
+    <col min="18" max="19" width="2.28515625" customWidth="1"/>
+    <col min="21" max="21" width="39.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="81" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="81"/>
       <c r="D1" s="35"/>
@@ -2425,7 +2429,7 @@
       <c r="G1" s="35"/>
       <c r="H1" s="35"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
       <c r="B2" s="30"/>
       <c r="D2" s="80" t="s">
@@ -2441,7 +2445,7 @@
       <c r="M2" s="69"/>
       <c r="N2" s="70"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
       <c r="B3" s="32"/>
       <c r="E3" s="80" t="s">
@@ -2453,7 +2457,7 @@
       <c r="J3" s="71"/>
       <c r="N3" s="67"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" s="32"/>
       <c r="D4" s="35"/>
@@ -2466,7 +2470,7 @@
       <c r="J4" s="71"/>
       <c r="N4" s="67"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="32"/>
       <c r="D5" s="79" t="s">
@@ -2480,7 +2484,7 @@
       <c r="N5" s="67"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="32"/>
       <c r="D6" s="80" t="s">
@@ -2492,7 +2496,7 @@
       <c r="J6" s="71"/>
       <c r="N6" s="67"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="32"/>
       <c r="D7" s="79" t="s">
@@ -2505,7 +2509,7 @@
       <c r="J7" s="71"/>
       <c r="N7" s="67"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="33"/>
       <c r="B8" s="34"/>
       <c r="D8" s="80" t="s">
@@ -2521,23 +2525,23 @@
       <c r="M8" s="73"/>
       <c r="N8" s="74"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="52" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="43.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="45.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
@@ -2581,13 +2585,13 @@
         <v>13</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="P13" s="78" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="41">
         <v>100</v>
       </c>
@@ -2640,12 +2644,12 @@
         <v>157.762</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="53" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="43.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="45.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
         <v>9</v>
       </c>
@@ -2689,13 +2693,13 @@
         <v>13</v>
       </c>
       <c r="O17" s="22" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26">
         <v>100</v>
       </c>
@@ -2772,25 +2776,25 @@
   </sheetPr>
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="7" width="9.83203125" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" customWidth="1"/>
-    <col min="9" max="14" width="9.83203125" customWidth="1"/>
-    <col min="15" max="15" width="17.83203125" customWidth="1"/>
-    <col min="16" max="16" width="14.83203125" customWidth="1"/>
-    <col min="17" max="17" width="14.1640625" customWidth="1"/>
-    <col min="18" max="18" width="3.1640625" customWidth="1"/>
+    <col min="1" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="14" width="9.85546875" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1"/>
+    <col min="18" max="18" width="3.140625" customWidth="1"/>
     <col min="19" max="19" width="3" customWidth="1"/>
     <col min="21" max="21" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="81" t="s">
         <v>26</v>
       </c>
@@ -2801,7 +2805,7 @@
       <c r="G1" s="35"/>
       <c r="H1" s="35"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
       <c r="B2" s="30"/>
       <c r="D2" s="80" t="s">
@@ -2817,7 +2821,7 @@
       <c r="M2" s="69"/>
       <c r="N2" s="70"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
       <c r="B3" s="32"/>
       <c r="E3" s="80" t="s">
@@ -2829,7 +2833,7 @@
       <c r="J3" s="71"/>
       <c r="N3" s="67"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
       <c r="B4" s="32"/>
       <c r="D4" s="35"/>
@@ -2842,7 +2846,7 @@
       <c r="J4" s="71"/>
       <c r="N4" s="67"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="32"/>
       <c r="D5" s="79" t="s">
@@ -2856,7 +2860,7 @@
       <c r="N5" s="67"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="32"/>
       <c r="D6" s="80" t="s">
@@ -2868,7 +2872,7 @@
       <c r="J6" s="71"/>
       <c r="N6" s="67"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="32"/>
       <c r="D7" s="79" t="s">
@@ -2881,7 +2885,7 @@
       <c r="J7" s="71"/>
       <c r="N7" s="67"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="33"/>
       <c r="B8" s="34"/>
       <c r="D8" s="80" t="s">
@@ -2897,18 +2901,18 @@
       <c r="M8" s="73"/>
       <c r="N8" s="74"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -2927,7 +2931,7 @@
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
-    <row r="13" spans="1:20" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="45.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
@@ -2974,10 +2978,10 @@
         <v>17</v>
       </c>
       <c r="P13" s="78" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="41">
         <v>100</v>
       </c>
@@ -3030,13 +3034,13 @@
         <v>175.65</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
         <v>6</v>
       </c>
       <c r="O16" s="11"/>
     </row>
-    <row r="17" spans="1:16" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="45.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
         <v>9</v>
       </c>
@@ -3080,13 +3084,13 @@
         <v>13</v>
       </c>
       <c r="O17" s="22" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26">
         <v>100</v>
       </c>

</xml_diff>